<commit_message>
Intégration du template et de la BDD au projet
</commit_message>
<xml_diff>
--- a/Documentation/Journaux_de_travail/AJT_TPI_Journal_de_travail.xlsx
+++ b/Documentation/Journaux_de_travail/AJT_TPI_Journal_de_travail.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\4ème année\TPI\Journal_de_travail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\4ème année\TPI_2019\Documentation\Journaux_de_travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -105,6 +105,27 @@
   </si>
   <si>
     <t>Finalisation du MCD et création du MLD.</t>
+  </si>
+  <si>
+    <t>Recherche d'un template pour le site web ainsi que d'une librairie pouvant gérer des graphiques, chart.js sera retenu.</t>
+  </si>
+  <si>
+    <t>Rédaction d'une partie de l'analyse de ma documentation.</t>
+  </si>
+  <si>
+    <t>Réinstallation et reconfiguration de wampserver dont plusieurs services ne fonctionnaient pas.</t>
+  </si>
+  <si>
+    <t>Lecture d'un exemple de Modele/Vue/Controlleur afin de réapprendre le fonctionnement de ce système pour pouvoir l'utiliser pour le site.</t>
+  </si>
+  <si>
+    <t>Adaptation du template trouvé au modèle MVC.</t>
+  </si>
+  <si>
+    <t>Création de la base de données et du script permettant de la créer automatiquement. Ajout d'une table "écoles" contenant la nom des écoles et ajout de la fonction créant toutes les écoles dans le script de création de la base de données.</t>
+  </si>
+  <si>
+    <t>Continuation de l'adaptation du template au modèle MVC avec l'aide d'un tutoriel vidéo.</t>
   </si>
 </sst>
 </file>
@@ -311,9 +332,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -329,12 +347,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -343,24 +379,6 @@
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -448,6 +466,9 @@
           <color indexed="64"/>
         </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -467,7 +488,7 @@
   <autoFilter ref="C30:D39"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Type"/>
-    <tableColumn id="2" name="Temps total" dataDxfId="1">
+    <tableColumn id="2" name="Temps total" dataDxfId="8">
       <calculatedColumnFormula>SUMIF(Tableau2[Type d''activité],C31,Tableau2[Temps nécessaire])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -476,13 +497,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:E25" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:E25" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B3:E25"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="4"/>
-    <tableColumn id="2" name="Type d'activité" dataDxfId="3"/>
-    <tableColumn id="3" name="Description de l'activité" dataDxfId="0"/>
-    <tableColumn id="4" name="Temps nécessaire" dataDxfId="2"/>
+    <tableColumn id="1" name="Date" dataDxfId="3"/>
+    <tableColumn id="2" name="Type d'activité" dataDxfId="2"/>
+    <tableColumn id="3" name="Description de l'activité" dataDxfId="1"/>
+    <tableColumn id="4" name="Temps nécessaire" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -756,8 +777,8 @@
   </sheetPr>
   <dimension ref="B3:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,13 +813,13 @@
       <c r="B4" s="9">
         <v>43592</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>2.5</v>
       </c>
     </row>
@@ -806,13 +827,13 @@
       <c r="B5" s="9">
         <v>43592</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>2</v>
       </c>
     </row>
@@ -820,13 +841,13 @@
       <c r="B6" s="9">
         <v>43592</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>1.5</v>
       </c>
     </row>
@@ -834,13 +855,13 @@
       <c r="B7" s="9">
         <v>43592</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>0.75</v>
       </c>
     </row>
@@ -848,13 +869,13 @@
       <c r="B8" s="9">
         <v>43593</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>1.5</v>
       </c>
     </row>
@@ -862,13 +883,13 @@
       <c r="B9" s="9">
         <v>43593</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>0.75</v>
       </c>
     </row>
@@ -876,13 +897,13 @@
       <c r="B10" s="9">
         <v>43594</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>0.75</v>
       </c>
     </row>
@@ -890,13 +911,13 @@
       <c r="B11" s="9">
         <v>43594</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <v>1.5</v>
       </c>
     </row>
@@ -904,13 +925,13 @@
       <c r="B12" s="9">
         <v>43594</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <v>0.75</v>
       </c>
     </row>
@@ -918,13 +939,13 @@
       <c r="B13" s="9">
         <v>43594</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
         <v>2.5</v>
       </c>
     </row>
@@ -932,81 +953,137 @@
       <c r="B14" s="9">
         <v>43594</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="13"/>
+    <row r="15" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
+        <v>43595</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="13">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="9">
+        <v>43595</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="9">
+        <v>43599</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="9">
+        <v>43599</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="13"/>
+      <c r="B19" s="9">
+        <v>43599</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="12">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B20" s="9">
+        <v>43599</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="9">
+        <v>43600</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="12">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="13"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="12"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="13"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="13"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="13"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="12"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
@@ -1022,7 +1099,7 @@
       </c>
       <c r="D31">
         <f>SUMIF(Tableau2[Type d''activité],C31,Tableau2[Temps nécessaire])</f>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
@@ -1031,7 +1108,7 @@
       </c>
       <c r="D32">
         <f>SUMIF(Tableau2[Type d''activité],C32,Tableau2[Temps nécessaire])</f>
-        <v>0</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
@@ -1040,7 +1117,7 @@
       </c>
       <c r="D33">
         <f>SUMIF(Tableau2[Type d''activité],C33,Tableau2[Temps nécessaire])</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
@@ -1067,7 +1144,7 @@
       </c>
       <c r="D36">
         <f>SUMIF(Tableau2[Type d''activité],C36,Tableau2[Temps nécessaire])</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
@@ -1103,7 +1180,7 @@
       </c>
       <c r="D41" s="4">
         <f>SUM(Table663[Temps total])</f>
-        <v>15</v>
+        <v>29.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sauvegarde du travail produit ce matin
</commit_message>
<xml_diff>
--- a/Documentation/Journaux_de_travail/AJT_TPI_Journal_de_travail.xlsx
+++ b/Documentation/Journaux_de_travail/AJT_TPI_Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Continuation de l'adaptation du template au modèle MVC avec l'aide d'un tutoriel vidéo.</t>
+  </si>
+  <si>
+    <t>Adaptation du template trouvé au modèle MVC. Création de l'accès à la page d'accueil. Cet accès n'est actuellement plus possible tant que je n'aurai pas résolu un problème de chargement de la bonne page.</t>
+  </si>
+  <si>
+    <t>Modification de mes entrées dans la base de données afin que celle-ci soient en anglais.</t>
   </si>
 </sst>
 </file>
@@ -777,8 +783,8 @@
   </sheetPr>
   <dimension ref="B3:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,17 +1067,33 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="12"/>
+    <row r="22" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B22" s="9">
+        <v>43632</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="9">
+        <v>43601</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
@@ -1117,7 +1139,7 @@
       </c>
       <c r="D33">
         <f>SUMIF(Tableau2[Type d''activité],C33,Tableau2[Temps nécessaire])</f>
-        <v>7.5</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
@@ -1180,7 +1202,7 @@
       </c>
       <c r="D41" s="4">
         <f>SUM(Table663[Temps total])</f>
-        <v>29.25</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sauvagarde du travail effectué sur l'inscription et la connexion
</commit_message>
<xml_diff>
--- a/Documentation/Journaux_de_travail/AJT_TPI_Journal_de_travail.xlsx
+++ b/Documentation/Journaux_de_travail/AJT_TPI_Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -132,6 +132,27 @@
   </si>
   <si>
     <t>Modification de mes entrées dans la base de données afin que celle-ci soient en anglais.</t>
+  </si>
+  <si>
+    <t>Correction des dernières erreurs des changements de pages.</t>
+  </si>
+  <si>
+    <t>Création de la page d'inscription.</t>
+  </si>
+  <si>
+    <t>Création de la page d'accueil et finalisation de la page événement. Cette tâche n'aurait pas dû être effectuée avant les pages d'inscirption et de connexion. Cependant, cela était nécessaire à ma bonne compréhension de mon modèle MVC, les tâches ont donc été inversées. Le retard que je semble avoir pris est bien moins important qu'il ne paraît.</t>
+  </si>
+  <si>
+    <t>Rassemblement des livrables oubliés et rédaction d'un mail à destination de mes experts ainsi que de mon chef de projet pour m'excuser de mon retard dans l'envoi de mes livrables.</t>
+  </si>
+  <si>
+    <t>Continuation de la documentation.</t>
+  </si>
+  <si>
+    <t>Finalisation de la page d'inscription</t>
+  </si>
+  <si>
+    <t>Ajout sur la page d'inscription d'une fonction allant chercher la liste des écoles dans ma base de données afin de limiter le choix d'entrée de l'utilisateur. Dû à des bugs et des problèmes de fonction, la réalisation de cette petite fonctionnalité m'a pris beaucoup de temps.</t>
   </si>
 </sst>
 </file>
@@ -490,12 +511,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table663" displayName="Table663" ref="C30:D39" totalsRowShown="0">
-  <autoFilter ref="C30:D39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table663" displayName="Table663" ref="C41:D50" totalsRowShown="0">
+  <autoFilter ref="C41:D50"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Type"/>
     <tableColumn id="2" name="Temps total" dataDxfId="8">
-      <calculatedColumnFormula>SUMIF(Tableau2[Type d''activité],C31,Tableau2[Temps nécessaire])</calculatedColumnFormula>
+      <calculatedColumnFormula>SUMIF(Tableau2[Type d''activité],C42,Tableau2[Temps nécessaire])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -503,8 +524,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:E25" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B3:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:E36" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B3:E36"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Date" dataDxfId="3"/>
     <tableColumn id="2" name="Type d'activité" dataDxfId="2"/>
@@ -781,10 +802,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:K41"/>
+  <dimension ref="B3:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,120 +1116,242 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="12"/>
+    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="9">
+        <v>43602</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B25" s="9">
+        <v>43602</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="9">
+        <v>43602</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B27" s="9">
+        <v>43606</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B28" s="9">
+        <v>43606</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="12">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="9">
+        <v>43606</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="12">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="B30" s="9">
+        <v>43606</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="12"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="12"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="12"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="12"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>13</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>7</v>
       </c>
-      <c r="D31">
-        <f>SUMIF(Tableau2[Type d''activité],C31,Tableau2[Temps nécessaire])</f>
+      <c r="D42">
+        <f>SUMIF(Tableau2[Type d''activité],C42,Tableau2[Temps nécessaire])</f>
         <v>10.25</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
         <v>15</v>
       </c>
-      <c r="D32">
-        <f>SUMIF(Tableau2[Type d''activité],C32,Tableau2[Temps nécessaire])</f>
+      <c r="D43">
+        <f>SUMIF(Tableau2[Type d''activité],C43,Tableau2[Temps nécessaire])</f>
         <v>3.75</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>16</v>
       </c>
-      <c r="D33">
-        <f>SUMIF(Tableau2[Type d''activité],C33,Tableau2[Temps nécessaire])</f>
-        <v>14.25</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+      <c r="D44">
+        <f>SUMIF(Tableau2[Type d''activité],C44,Tableau2[Temps nécessaire])</f>
+        <v>15.75</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
         <v>9</v>
       </c>
-      <c r="D34">
-        <f>SUMIF(Tableau2[Type d''activité],C34,Tableau2[Temps nécessaire])</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+      <c r="D45">
+        <f>SUMIF(Tableau2[Type d''activité],C45,Tableau2[Temps nécessaire])</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
         <v>17</v>
       </c>
-      <c r="D35">
-        <f>SUMIF(Tableau2[Type d''activité],C35,Tableau2[Temps nécessaire])</f>
+      <c r="D46">
+        <f>SUMIF(Tableau2[Type d''activité],C46,Tableau2[Temps nécessaire])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <f>SUMIF(Tableau2[Type d''activité],C47,Tableau2[Temps nécessaire])</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48">
+        <f>SUMIF(Tableau2[Type d''activité],C48,Tableau2[Temps nécessaire])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36">
-        <f>SUMIF(Tableau2[Type d''activité],C36,Tableau2[Temps nécessaire])</f>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37">
-        <f>SUMIF(Tableau2[Type d''activité],C37,Tableau2[Temps nécessaire])</f>
+      <c r="D49">
+        <f>SUMIF(Tableau2[Type d''activité],C49,Tableau2[Temps nécessaire])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50">
+        <f>SUMIF(Tableau2[Type d''activité],C50,Tableau2[Temps nécessaire])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38">
-        <f>SUMIF(Tableau2[Type d''activité],C38,Tableau2[Temps nécessaire])</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39">
-        <f>SUMIF(Tableau2[Type d''activité],C39,Tableau2[Temps nécessaire])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="4" t="s">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D52" s="4">
         <f>SUM(Table663[Temps total])</f>
-        <v>36</v>
+        <v>46.5</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C25">
-      <formula1>$C$31:$C$39</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C36">
+      <formula1>$C$42:$C$50</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Affichage des utilisateurs dans la partie administration
</commit_message>
<xml_diff>
--- a/Documentation/Journaux_de_travail/AJT_TPI_Journal_de_travail.xlsx
+++ b/Documentation/Journaux_de_travail/AJT_TPI_Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -155,7 +155,19 @@
     <t>Ajout sur la page d'inscription d'une fonction allant chercher la liste des écoles dans ma base de données afin de limiter le choix d'entrée de l'utilisateur. Dû à des bugs et des problèmes de fonction, la réalisation de cette petite fonctionnalité m'a pris beaucoup de temps.</t>
   </si>
   <si>
-    <t>…</t>
+    <t>Restructuration de mon MVC, ajout de la fonction d'inscription, création de la page de login, ajout de la fonction de login et de logout avec une variable session vidée proprement. Mise en forme d'éléments CSS.</t>
+  </si>
+  <si>
+    <t>Création d'une fonction de vérification de compléxité de mot de passe. Fonction mise de côté pour le moment dû à son non-fonctionnement pour une raison qui m'est pour l'instant inconnue.</t>
+  </si>
+  <si>
+    <t>Visite du deuxième expert, discussion de l'état actuel du projet et des prochaines étapes.</t>
+  </si>
+  <si>
+    <t>Discussion de l'état actuel du projet et des prochaines étapes avec mon chef de projet.</t>
+  </si>
+  <si>
+    <t>Création d'une condition d'affiche en fonction du type d'utilisateur connecté (admin ou non), création de la page admin et ajout de contenu sur celle-ci. J'ai reçu l'aide d'un collègue durant environ ~15 minutes.</t>
   </si>
 </sst>
 </file>
@@ -514,12 +526,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table663" displayName="Table663" ref="C41:D50" totalsRowShown="0">
-  <autoFilter ref="C41:D50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table663" displayName="Table663" ref="C47:D56" totalsRowShown="0">
+  <autoFilter ref="C47:D56"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Type"/>
     <tableColumn id="2" name="Temps total" dataDxfId="8">
-      <calculatedColumnFormula>SUMIF(Tableau2[Type d''activité],C42,Tableau2[Temps nécessaire])</calculatedColumnFormula>
+      <calculatedColumnFormula>SUMIF(Tableau2[Type d''activité],C48,Tableau2[Temps nécessaire])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -527,8 +539,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:E36" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B3:E36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:E42" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B3:E42"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Date" dataDxfId="3"/>
     <tableColumn id="2" name="Type d'activité" dataDxfId="2"/>
@@ -805,10 +817,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:K52"/>
+  <dimension ref="B3:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1243,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>43608</v>
       </c>
@@ -1245,132 +1257,200 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="12"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="12"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="12"/>
+    <row r="33" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B33" s="9">
+        <v>43609</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="12">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="9">
+        <v>43609</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B35" s="9">
+        <v>43609</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="9">
+        <v>43609</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="12"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="10"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="10"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="10"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="12"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" t="s">
-        <v>14</v>
-      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="12"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42">
-        <f>SUMIF(Tableau2[Type d''activité],C42,Tableau2[Temps nécessaire])</f>
-        <v>10.25</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43">
-        <f>SUMIF(Tableau2[Type d''activité],C43,Tableau2[Temps nécessaire])</f>
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44">
-        <f>SUMIF(Tableau2[Type d''activité],C44,Tableau2[Temps nécessaire])</f>
-        <v>15.75</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45">
-        <f>SUMIF(Tableau2[Type d''activité],C45,Tableau2[Temps nécessaire])</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46">
-        <f>SUMIF(Tableau2[Type d''activité],C46,Tableau2[Temps nécessaire])</f>
-        <v>13.75</v>
-      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="12"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47">
-        <f>SUMIF(Tableau2[Type d''activité],C47,Tableau2[Temps nécessaire])</f>
-        <v>5.5</v>
+        <v>13</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D48">
         <f>SUMIF(Tableau2[Type d''activité],C48,Tableau2[Temps nécessaire])</f>
-        <v>0</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D49">
         <f>SUMIF(Tableau2[Type d''activité],C49,Tableau2[Temps nécessaire])</f>
-        <v>2</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D50">
         <f>SUMIF(Tableau2[Type d''activité],C50,Tableau2[Temps nécessaire])</f>
+        <v>15.75</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51">
+        <f>SUMIF(Tableau2[Type d''activité],C51,Tableau2[Temps nécessaire])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52">
+        <f>SUMIF(Tableau2[Type d''activité],C52,Tableau2[Temps nécessaire])</f>
+        <v>17.75</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <f>SUMIF(Tableau2[Type d''activité],C53,Tableau2[Temps nécessaire])</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54">
+        <f>SUMIF(Tableau2[Type d''activité],C54,Tableau2[Temps nécessaire])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="4" t="s">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <f>SUMIF(Tableau2[Type d''activité],C55,Tableau2[Temps nécessaire])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56">
+        <f>SUMIF(Tableau2[Type d''activité],C56,Tableau2[Temps nécessaire])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D58" s="4">
         <f>SUM(Table663[Temps total])</f>
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C36">
-      <formula1>$C$42:$C$50</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C42">
+      <formula1>$C$48:$C$56</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout de la fonction de visualisation des ateliers et correction des erreurs
</commit_message>
<xml_diff>
--- a/Documentation/Journaux_de_travail/AJT_TPI_Journal_de_travail.xlsx
+++ b/Documentation/Journaux_de_travail/AJT_TPI_Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -168,6 +168,21 @@
   </si>
   <si>
     <t>Création d'une condition d'affiche en fonction du type d'utilisateur connecté (admin ou non), création de la page admin et ajout de contenu sur celle-ci. J'ai reçu l'aide d'un collègue durant environ ~15 minutes.</t>
+  </si>
+  <si>
+    <t>Ajout de la fonction d'affichage des utilisateurs pour les administrateurs.</t>
+  </si>
+  <si>
+    <t>Ajout de la fonction de suppression des utilisateurs pour les administrateurs.</t>
+  </si>
+  <si>
+    <t>Ajout de la fonction d'affichage des événements pour les administrateurs.</t>
+  </si>
+  <si>
+    <t>Ajout de la fonction de modification des événements pour les administrateurs.</t>
+  </si>
+  <si>
+    <t>Commencement de la fonction d'affichage des ateliers par événements.</t>
   </si>
 </sst>
 </file>
@@ -526,12 +541,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table663" displayName="Table663" ref="C47:D56" totalsRowShown="0">
-  <autoFilter ref="C47:D56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table663" displayName="Table663" ref="C51:D60" totalsRowShown="0">
+  <autoFilter ref="C51:D60"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Type"/>
     <tableColumn id="2" name="Temps total" dataDxfId="8">
-      <calculatedColumnFormula>SUMIF(Tableau2[Type d''activité],C48,Tableau2[Temps nécessaire])</calculatedColumnFormula>
+      <calculatedColumnFormula>SUMIF(Tableau2[Type d''activité],C52,Tableau2[Temps nécessaire])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -539,8 +554,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:E42" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B3:E42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:E46" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B3:E46"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Date" dataDxfId="3"/>
     <tableColumn id="2" name="Type d'activité" dataDxfId="2"/>
@@ -817,10 +832,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:K58"/>
+  <dimension ref="B3:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,144 +1328,208 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="10"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="12"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="10"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="12"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="12"/>
+    <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="9">
+        <v>43613</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="9">
+        <v>43613</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39" s="9">
+        <v>43613</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="9">
+        <v>43613</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="9">
+        <v>43613</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="12">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
+      <c r="B42" s="9"/>
       <c r="C42" s="11"/>
       <c r="D42" s="14"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48">
-        <f>SUMIF(Tableau2[Type d''activité],C48,Tableau2[Temps nécessaire])</f>
-        <v>10.25</v>
-      </c>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49">
-        <f>SUMIF(Tableau2[Type d''activité],C49,Tableau2[Temps nécessaire])</f>
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50">
-        <f>SUMIF(Tableau2[Type d''activité],C50,Tableau2[Temps nécessaire])</f>
-        <v>15.75</v>
-      </c>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="9"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="12"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="9"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="12"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="9"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="12"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="10"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="12"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51">
-        <f>SUMIF(Tableau2[Type d''activité],C51,Tableau2[Temps nécessaire])</f>
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D52">
         <f>SUMIF(Tableau2[Type d''activité],C52,Tableau2[Temps nécessaire])</f>
-        <v>17.75</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D53">
         <f>SUMIF(Tableau2[Type d''activité],C53,Tableau2[Temps nécessaire])</f>
-        <v>6.5</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D54">
         <f>SUMIF(Tableau2[Type d''activité],C54,Tableau2[Temps nécessaire])</f>
-        <v>0</v>
+        <v>15.75</v>
       </c>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D55">
         <f>SUMIF(Tableau2[Type d''activité],C55,Tableau2[Temps nécessaire])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D56">
         <f>SUMIF(Tableau2[Type d''activité],C56,Tableau2[Temps nécessaire])</f>
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <f>SUMIF(Tableau2[Type d''activité],C57,Tableau2[Temps nécessaire])</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58">
+        <f>SUMIF(Tableau2[Type d''activité],C58,Tableau2[Temps nécessaire])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="4" t="s">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59">
+        <f>SUMIF(Tableau2[Type d''activité],C59,Tableau2[Temps nécessaire])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60">
+        <f>SUMIF(Tableau2[Type d''activité],C60,Tableau2[Temps nécessaire])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D62" s="4">
         <f>SUM(Table663[Temps total])</f>
-        <v>59</v>
+        <v>65.75</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C42">
-      <formula1>$C$48:$C$56</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C46">
+      <formula1>$C$52:$C$60</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>